<commit_message>
ADC works. Button working well. BOM and Schematic change
Button works better with 10k pull up and 100k in series with UVLO
blocking diode. The schematic and BOM have been updated.

There's code (in Application.c for now) that monitors VBat line and
turns the micro off when the voltage drops below 3.2v.

There's code for the soft power-off in application.c too.
</commit_message>
<xml_diff>
--- a/Circuit/R6_1/allegro_c6r3/CM Files/C6R3_BOM.xlsx
+++ b/Circuit/R6_1/allegro_c6r3/CM Files/C6R3_BOM.xlsx
@@ -497,9 +497,6 @@
     <t>CRCW040230R0FKED</t>
   </si>
   <si>
-    <t>R5 R10 R11 R16 R17 R18 R19 R23 R24 R25 R31 R33</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -560,9 +557,6 @@
     <t>CRCW040222K0FKED</t>
   </si>
   <si>
-    <t>R14 R28 R29 R32 R34</t>
-  </si>
-  <si>
     <t>100k</t>
   </si>
   <si>
@@ -831,6 +825,12 @@
   </si>
   <si>
     <t>MM3Z3V3ST1G</t>
+  </si>
+  <si>
+    <t>R14 R28 R29 R33 R34</t>
+  </si>
+  <si>
+    <t>R5 R10 R11 R16 R17 R18 R19 R23 R24 R25 R31 R32</t>
   </si>
 </sst>
 </file>
@@ -1161,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,22 +1273,22 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>151</v>
@@ -1360,22 +1360,22 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>151</v>
@@ -1389,22 +1389,22 @@
         <v>12</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>151</v>
@@ -1476,22 +1476,22 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>151</v>
@@ -1534,25 +1534,25 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1563,22 +1563,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>151</v>
@@ -1737,22 +1737,22 @@
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>151</v>
@@ -1766,22 +1766,22 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>151</v>
@@ -1853,25 +1853,25 @@
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="F24" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="I24" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1911,22 +1911,22 @@
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>151</v>
@@ -1998,25 +1998,25 @@
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="I29" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2201,22 +2201,22 @@
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>151</v>
@@ -2259,25 +2259,25 @@
         <v>1</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2288,25 +2288,25 @@
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="G39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2317,25 +2317,25 @@
         <v>1</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="G40" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2346,25 +2346,25 @@
         <v>1</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="G41" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2404,25 +2404,25 @@
         <v>1</v>
       </c>
       <c r="C43" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="G43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2462,25 +2462,25 @@
         <v>1</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="G45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2491,22 +2491,22 @@
         <v>1</v>
       </c>
       <c r="C46" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>75</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>145</v>
@@ -2520,25 +2520,25 @@
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="G47" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2549,25 +2549,25 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="G48" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2665,25 +2665,25 @@
         <v>1</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="G52" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2694,25 +2694,25 @@
         <v>1</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="G53" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>